<commit_message>
Update new Lambda and SNS checks with compliance requirements
Update new Lambda and SNS checks with compliance requirements via Compliance.RelatedRequirements in both Comm. and GovCloud. Fixed ASFF parameters for workflow and record state in SNS. Fixed formatting in the markdown table in core readme. Updated Compliance mapping Excel and added CSV version
</commit_message>
<xml_diff>
--- a/compliance-mapping/electriceye-auditor-compliance-mapping.xlsx
+++ b/compliance-mapping/electriceye-auditor-compliance-mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\Cloud Stuff\ElectricEye\NIST CSF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\ElectricEye\compliance-mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7278E176-BA12-4544-8F29-03CB7BD213C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9262D57-73D2-447D-8BAB-0BDDD69AB358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CF00DBA1-7D00-4BAF-9CDB-2D555C965A45}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="405">
   <si>
     <t>Auditor File Name</t>
   </si>
@@ -1259,6 +1259,21 @@
   </si>
   <si>
     <t>NIST SP 800-53 AC-1, NIST SP 800-53 AC-2, NIST SP 800-53 AC-3, NIST SP 800-53 AC-5, NIST SP 800-53 AC-6, NIST SP 800-53 AC-14, NIST SP 800-53 AC-16, NIST SP 800-53 AC-24</t>
+  </si>
+  <si>
+    <t>Does the topic allow public access</t>
+  </si>
+  <si>
+    <t>Does the topic allow cross-account access</t>
+  </si>
+  <si>
+    <t>AWS_Lambda_Auditor.py</t>
+  </si>
+  <si>
+    <t>Lambda function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has function been used or updated in the last 30 days </t>
   </si>
 </sst>
 </file>
@@ -1665,11 +1680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FE6E02-AA90-4307-B05B-28AB6738FE85}">
-  <dimension ref="A1:G211"/>
+  <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D199" sqref="D199:G199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5110,96 +5125,96 @@
         <v>388</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>193</v>
+        <v>400</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>378</v>
+        <v>288</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>379</v>
+        <v>319</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B152" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C152" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D151" s="2" t="s">
+      <c r="D153" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="E151" s="4" t="s">
+      <c r="E153" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="F151" s="2" t="s">
+      <c r="F153" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="G151" s="2" t="s">
+      <c r="G153" s="2" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G152" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F153" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G153" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5210,99 +5225,99 @@
         <v>196</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="G154" s="6" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G156" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B157" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C157" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D155" s="2" t="s">
+      <c r="D157" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="E155" s="2" t="s">
+      <c r="E157" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="F155" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G155" s="2" t="s">
+      <c r="F157" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G157" s="2" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G156" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G157" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>288</v>
@@ -5317,27 +5332,27 @@
         <v>319</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>350</v>
+        <v>204</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>353</v>
+        <v>312</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>307</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5345,22 +5360,22 @@
         <v>205</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>351</v>
+        <v>207</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>353</v>
+        <v>288</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5371,65 +5386,65 @@
         <v>208</v>
       </c>
       <c r="C161" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G162" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D161" s="2" t="s">
+      <c r="D163" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="E161" s="4" t="s">
+      <c r="E163" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="F161" s="2" t="s">
+      <c r="F163" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="G161" s="2" t="s">
+      <c r="G163" s="2" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="G163" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5437,10 +5452,10 @@
         <v>209</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>212</v>
+        <v>44</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>289</v>
@@ -5460,10 +5475,10 @@
         <v>209</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>289</v>
@@ -5483,10 +5498,10 @@
         <v>209</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>289</v>
@@ -5503,82 +5518,82 @@
     </row>
     <row r="167" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G167" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B169" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C169" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D167" s="2" t="s">
+      <c r="D169" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E167" s="2" t="s">
+      <c r="E169" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F167" s="2" t="s">
+      <c r="F169" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="G167" s="2" t="s">
+      <c r="G169" s="2" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E168" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G168" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>338</v>
@@ -5593,7 +5608,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>220</v>
       </c>
@@ -5601,19 +5616,19 @@
         <v>221</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>371</v>
+        <v>338</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5624,7 +5639,7 @@
         <v>221</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>338</v>
@@ -5639,7 +5654,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>220</v>
       </c>
@@ -5647,68 +5662,68 @@
         <v>221</v>
       </c>
       <c r="C173" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G173" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G174" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C175" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D173" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E173" s="2" t="s">
+      <c r="E175" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="F173" s="2" t="s">
+      <c r="F175" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="G173" s="2" t="s">
+      <c r="G175" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F174" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G174" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E175" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="F175" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G175" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>227</v>
       </c>
@@ -5716,22 +5731,22 @@
         <v>228</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>334</v>
+        <v>229</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>227</v>
       </c>
@@ -5739,22 +5754,22 @@
         <v>228</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>371</v>
+        <v>352</v>
+      </c>
+      <c r="E177" s="4" t="s">
+        <v>353</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>307</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>227</v>
       </c>
@@ -5762,53 +5777,53 @@
         <v>228</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>232</v>
+        <v>334</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E178" s="4" t="s">
-        <v>340</v>
+        <v>306</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>341</v>
+        <v>310</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>368</v>
+        <v>312</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>307</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>369</v>
+        <v>320</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>338</v>
@@ -5823,53 +5838,53 @@
         <v>339</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>288</v>
+        <v>368</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E182" s="2" t="s">
-        <v>370</v>
+        <v>338</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="G182" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="G182" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>236</v>
       </c>
@@ -5877,65 +5892,65 @@
         <v>237</v>
       </c>
       <c r="C183" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G183" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G184" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C185" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D183" s="2" t="s">
+      <c r="D185" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E183" s="2" t="s">
+      <c r="E185" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F183" s="2" t="s">
+      <c r="F185" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="G183" s="2" t="s">
+      <c r="G185" s="2" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D184" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F184" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G184" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E185" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F185" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G185" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5946,7 +5961,7 @@
         <v>242</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>311</v>
+        <v>243</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>312</v>
@@ -5966,10 +5981,10 @@
         <v>241</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>312</v>
@@ -5989,10 +6004,10 @@
         <v>241</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>312</v>
@@ -6007,7 +6022,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>241</v>
       </c>
@@ -6015,65 +6030,65 @@
         <v>245</v>
       </c>
       <c r="C189" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G190" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C191" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D189" s="2" t="s">
+      <c r="D191" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E189" s="2" t="s">
+      <c r="E191" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F189" s="2" t="s">
+      <c r="F191" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="G189" s="2" t="s">
+      <c r="G191" s="2" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E190" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F190" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G190" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D191" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E191" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F191" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G191" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -6081,10 +6096,10 @@
         <v>249</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>306</v>
@@ -6099,7 +6114,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>249</v>
       </c>
@@ -6107,19 +6122,19 @@
         <v>252</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>306</v>
+        <v>389</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>373</v>
+        <v>399</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -6130,7 +6145,7 @@
         <v>252</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>306</v>
@@ -6150,10 +6165,10 @@
         <v>249</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>302</v>
+        <v>255</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>306</v>
@@ -6173,10 +6188,10 @@
         <v>249</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>306</v>
@@ -6191,153 +6206,153 @@
         <v>394</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>306</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G198" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G199" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B199" s="3" t="s">
+      <c r="B201" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C199" s="3" t="s">
+      <c r="C201" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C202" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D199" s="2" t="s">
+      <c r="D202" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E199" s="2" t="s">
+      <c r="E202" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F199" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G199" s="2" t="s">
+      <c r="F202" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G202" s="2" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E200" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F200" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G200" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F201" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G201" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A202" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E202" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F202" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G202" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>326</v>
@@ -6352,73 +6367,73 @@
         <v>328</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>44</v>
+        <v>269</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>376</v>
+        <v>327</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G204" s="5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>103</v>
+        <v>271</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>376</v>
+        <v>327</v>
       </c>
       <c r="F205" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G205" s="5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="G205" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>376</v>
+        <v>327</v>
       </c>
       <c r="F206" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G206" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="207" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6426,10 +6441,10 @@
         <v>275</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>324</v>
@@ -6449,10 +6464,10 @@
         <v>275</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>281</v>
+        <v>103</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>324</v>
@@ -6472,10 +6487,10 @@
         <v>275</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>324</v>
@@ -6495,10 +6510,10 @@
         <v>275</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>324</v>
@@ -6513,16 +6528,85 @@
         <v>325</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A211" s="7"/>
-      <c r="B211" s="7"/>
-      <c r="C211" s="7"/>
-      <c r="D211" s="5"/>
-      <c r="E211" s="7"/>
+    <row r="211" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="F211" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="G211" s="7"/>
+      <c r="G211" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G212" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G213" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214" s="7"/>
+      <c r="B214" s="7"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="5"/>
+      <c r="E214" s="7"/>
+      <c r="F214" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G214" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>